<commit_message>
added auto save of html to local
</commit_message>
<xml_diff>
--- a/eval/auto_eval/top_3_configurations.xlsx
+++ b/eval/auto_eval/top_3_configurations.xlsx
@@ -525,11 +525,11 @@
         <v>8000</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>text-embedding-ada-002</t>
+          <t>('bge-large', 'bge-large-en-v1.5', 1024)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -538,10 +538,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>4.2</v>
+        <v>3.8</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
@@ -550,10 +550,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="K2" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L2" t="n">
         <v>1.8</v>
@@ -563,12 +563,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>/Users/yonghuizhu/imperial/contoso-chat-backend/eval/auto_eval/meta_llama3_instruct_70B_top0.9_embtext-embedding-ada-002_originaltemplate.ipynb</t>
+          <t>/Users/yonghuizhu/imperial/contoso-chat-backend/eval/auto_eval/meta_llama3_instruct_70B_top0.5_emb('bge-large', 'bge-large-en-v1.5', 1024)_originaltemplate.ipynb</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2024_06_19_131434chat_eval_run</t>
+          <t>2024_06_19_155426chat_eval_run</t>
         </is>
       </c>
       <c r="P2" t="n">
@@ -578,18 +578,18 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>meta_llama3_instruct_70B</t>
+          <t>Phi_3_mini_4k_instruct</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>text-embedding-ada-002</t>
+          <t>['bge-large', 'bge-large-en-v1.5', 1024]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -598,54 +598,54 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="G3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="K3" t="n">
         <v>60</v>
       </c>
-      <c r="H3" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="I3" t="n">
-        <v>60</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="K3" t="n">
-        <v>20</v>
-      </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>/Users/yonghuizhu/imperial/contoso-chat-backend/eval/auto_eval/meta_llama3_instruct_70B_top0.5_embtext-embedding-ada-002_originaltemplate.ipynb</t>
+          <t>/Users/yonghuizhu/imperial/contoso-chat-backend/eval/auto_eval/Phi_3_mini_4k_instruct_top0.5_emb['bge-large', 'bge-large-en-v1.5', 1024]_originaltemplate.ipynb</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2024_06_19_130923chat_eval_run</t>
+          <t>2024_06_19_152518chat_eval_run</t>
         </is>
       </c>
       <c r="P3" t="n">
-        <v>16.28</v>
+        <v>18.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Phi_3_mini_4k_instruct</t>
+          <t>meta_llama3_instruct_70B</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -658,10 +658,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="G4" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="K4" t="n">
         <v>60</v>
@@ -683,16 +683,16 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>/Users/yonghuizhu/imperial/contoso-chat-backend/eval/auto_eval/Phi_3_mini_4k_instruct_top0.5_embtext-embedding-ada-002_originaltemplate.ipynb</t>
+          <t>/Users/yonghuizhu/imperial/contoso-chat-backend/eval/auto_eval/meta_llama3_instruct_70B_top0.9_embtext-embedding-ada-002_originaltemplate.ipynb</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2024_06_19_115233chat_eval_run</t>
+          <t>2024_06_19_131434chat_eval_run</t>
         </is>
       </c>
       <c r="P4" t="n">
-        <v>13.84</v>
+        <v>18.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>